<commit_message>
FW 0.1 - temp sensor
</commit_message>
<xml_diff>
--- a/sw/CAN_Adresses.xlsx
+++ b/sw/CAN_Adresses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t xml:space="preserve">SID bits</t>
   </si>
@@ -279,15 +279,6 @@
     <t xml:space="preserve">Force clear all addresses</t>
   </si>
   <si>
-    <t xml:space="preserve">Get node status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get node MCU temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get node uptime</t>
-  </si>
-  <si>
     <t xml:space="preserve">Peripherial specific commands</t>
   </si>
   <si>
@@ -381,6 +372,21 @@
     <t xml:space="preserve">Uptime in ms - 7 bytes</t>
   </si>
   <si>
+    <t>CAN_TM_GET_FW_VER_RES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get firmware version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FW Major</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FW Minor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peripherial specific commands - temperature sensor</t>
   </si>
   <si>
@@ -438,10 +444,25 @@
     <t>CAN_TS_GET_STATUS</t>
   </si>
   <si>
+    <t xml:space="preserve">Get node status</t>
+  </si>
+  <si>
     <t>CAN_TS_GET_TEMP</t>
   </si>
   <si>
+    <t xml:space="preserve">Get node MCU temperature</t>
+  </si>
+  <si>
     <t>CAN_TS_GET_UPTIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get node uptime</t>
+  </si>
+  <si>
+    <t>CAN_TS_GET_FW_VER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get firmware verison</t>
   </si>
   <si>
     <t xml:space="preserve">Peripherial specific commands - tempretarure sensor</t>
@@ -626,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -688,6 +709,7 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2141,7 +2163,7 @@
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -2167,7 +2189,7 @@
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -2193,7 +2215,7 @@
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -5317,7 +5339,7 @@
     </row>
     <row r="139">
       <c r="A139" s="16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B139" s="16"/>
       <c r="C139" s="16"/>
@@ -5357,7 +5379,7 @@
     </row>
     <row r="141">
       <c r="A141" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
@@ -5378,7 +5400,7 @@
         <v>255</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C142" s="12">
         <v>11111111</v>
@@ -8906,7 +8928,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8918,12 +8940,14 @@
     <col customWidth="1" min="4" max="4" width="34.28125"/>
     <col customWidth="1" min="5" max="5" width="39.140625"/>
     <col customWidth="1" min="7" max="7" width="18.57421875"/>
-    <col customWidth="1" min="8" max="8" width="18.8515625"/>
+    <col customWidth="1" min="8" max="8" width="13.140625"/>
+    <col customWidth="1" min="9" max="9" width="10.421875"/>
+    <col customWidth="1" min="10" max="11" width="11.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="21">
       <c r="A1" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -8948,13 +8972,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>56</v>
@@ -8962,7 +8986,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5"/>
@@ -8974,7 +8998,7 @@
     <row r="7"/>
     <row r="8" s="2" customFormat="1">
       <c r="A8" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>60</v>
@@ -9048,16 +9072,16 @@
         <v>00000000</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F10" s="18">
         <v>1</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="10"/>
@@ -9080,16 +9104,16 @@
         <v>00000001</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F11" s="20">
         <v>1</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="12"/>
@@ -9112,16 +9136,16 @@
         <v>00000010</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F12" s="20">
         <v>1</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="12"/>
@@ -9144,16 +9168,16 @@
         <v>00000011</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F13" s="20">
         <v>1</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="12"/>
@@ -9176,19 +9200,19 @@
         <v>00000100</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F14" s="20">
         <v>5</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
@@ -9210,19 +9234,19 @@
         <v>00000101</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F15" s="20">
         <v>2</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -9244,19 +9268,19 @@
         <v>00000110</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F16" s="20">
         <v>2</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -9278,19 +9302,19 @@
         <v>00000111</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F17" s="20">
         <v>2</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -9312,19 +9336,19 @@
         <v>00001000</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F18" s="20">
         <v>8</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="24"/>
@@ -9345,15 +9369,27 @@
         <f t="shared" si="7"/>
         <v>00001001</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="D19" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="12">
+        <v>4</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>122</v>
+      </c>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
@@ -12445,7 +12481,7 @@
     </row>
     <row r="139">
       <c r="A139" s="16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B139" s="16"/>
       <c r="C139" s="16"/>
@@ -12471,17 +12507,17 @@
       <c r="C140" s="12">
         <v>10000000</v>
       </c>
-      <c r="D140" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="E140" s="26" t="s">
-        <v>123</v>
+      <c r="D140" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E140" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="F140" s="20">
         <v>1</v>
       </c>
       <c r="G140" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H140" s="12"/>
       <c r="I140" s="12"/>
@@ -12493,7 +12529,7 @@
     </row>
     <row r="141">
       <c r="A141" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
@@ -12514,7 +12550,7 @@
         <v>255</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C142" s="12">
         <v>11111111</v>
@@ -16042,7 +16078,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -16058,7 +16094,7 @@
   <sheetData>
     <row r="1" ht="21">
       <c r="A1" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -16083,7 +16119,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -16097,7 +16133,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5"/>
@@ -16182,16 +16218,16 @@
         <v>00000000</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -16214,16 +16250,16 @@
         <v>00000001</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F11" s="12">
         <v>1</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -16246,19 +16282,19 @@
         <v>00000010</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F12" s="12">
         <v>2</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -16280,16 +16316,16 @@
         <v>00000011</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F13" s="12">
         <v>1</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -16312,16 +16348,16 @@
         <v>00000100</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F14" s="20">
         <v>1</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -16344,16 +16380,16 @@
         <v>00000101</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F15" s="20">
         <v>1</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -16376,16 +16412,16 @@
         <v>00000110</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="F16" s="20">
         <v>1</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -16408,16 +16444,16 @@
         <v>00000111</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="F17" s="20">
         <v>1</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -16440,16 +16476,16 @@
         <v>00001000</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>89</v>
+        <v>146</v>
       </c>
       <c r="F18" s="20">
         <v>1</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -16471,15 +16507,17 @@
         <f t="shared" si="13"/>
         <v>00001001</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12" t="s">
-        <v>33</v>
+      <c r="D19" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>148</v>
       </c>
       <c r="F19" s="20">
         <v>1</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -16509,7 +16547,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -16539,7 +16577,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -16569,7 +16607,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -16599,7 +16637,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -16629,7 +16667,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -16659,7 +16697,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -16689,7 +16727,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -16719,7 +16757,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -16749,7 +16787,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -16779,7 +16817,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -16809,7 +16847,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -16839,7 +16877,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -16869,7 +16907,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -16899,7 +16937,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
@@ -16929,7 +16967,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
@@ -16959,7 +16997,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
@@ -16989,7 +17027,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
@@ -17019,7 +17057,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
@@ -17049,7 +17087,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
@@ -17079,7 +17117,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
@@ -17109,7 +17147,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
@@ -17139,7 +17177,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
@@ -17169,7 +17207,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
@@ -17199,7 +17237,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
@@ -17229,7 +17267,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
@@ -17259,7 +17297,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
@@ -17289,7 +17327,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
@@ -17319,7 +17357,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
@@ -17349,7 +17387,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
@@ -17379,7 +17417,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
@@ -17409,7 +17447,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
@@ -17439,7 +17477,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
@@ -17469,7 +17507,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
@@ -17499,7 +17537,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
@@ -17529,7 +17567,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
@@ -17559,7 +17597,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
@@ -17589,7 +17627,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
@@ -17619,7 +17657,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
@@ -17649,7 +17687,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
@@ -17679,7 +17717,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
@@ -17709,7 +17747,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
@@ -17739,7 +17777,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
@@ -17769,7 +17807,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
@@ -17799,7 +17837,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H63" s="12"/>
       <c r="I63" s="12"/>
@@ -17829,7 +17867,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H64" s="12"/>
       <c r="I64" s="12"/>
@@ -17859,7 +17897,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
@@ -17889,7 +17927,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
@@ -17919,7 +17957,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
@@ -17949,7 +17987,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H68" s="12"/>
       <c r="I68" s="12"/>
@@ -17979,7 +18017,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
@@ -18009,7 +18047,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H70" s="12"/>
       <c r="I70" s="12"/>
@@ -18039,7 +18077,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="12"/>
@@ -18069,7 +18107,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H72" s="12"/>
       <c r="I72" s="12"/>
@@ -18099,7 +18137,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H73" s="12"/>
       <c r="I73" s="12"/>
@@ -18129,7 +18167,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H74" s="12"/>
       <c r="I74" s="12"/>
@@ -18159,7 +18197,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H75" s="12"/>
       <c r="I75" s="12"/>
@@ -18189,7 +18227,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H76" s="12"/>
       <c r="I76" s="12"/>
@@ -18219,7 +18257,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H77" s="12"/>
       <c r="I77" s="12"/>
@@ -18249,7 +18287,7 @@
         <v>1</v>
       </c>
       <c r="G78" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H78" s="12"/>
       <c r="I78" s="12"/>
@@ -18279,7 +18317,7 @@
         <v>1</v>
       </c>
       <c r="G79" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
@@ -18309,7 +18347,7 @@
         <v>1</v>
       </c>
       <c r="G80" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H80" s="12"/>
       <c r="I80" s="12"/>
@@ -18339,7 +18377,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H81" s="12"/>
       <c r="I81" s="12"/>
@@ -18369,7 +18407,7 @@
         <v>1</v>
       </c>
       <c r="G82" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H82" s="12"/>
       <c r="I82" s="12"/>
@@ -18399,7 +18437,7 @@
         <v>1</v>
       </c>
       <c r="G83" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="12"/>
@@ -18429,7 +18467,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="12"/>
@@ -18459,7 +18497,7 @@
         <v>1</v>
       </c>
       <c r="G85" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H85" s="12"/>
       <c r="I85" s="12"/>
@@ -18489,7 +18527,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H86" s="12"/>
       <c r="I86" s="12"/>
@@ -18519,7 +18557,7 @@
         <v>1</v>
       </c>
       <c r="G87" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H87" s="12"/>
       <c r="I87" s="12"/>
@@ -18549,7 +18587,7 @@
         <v>1</v>
       </c>
       <c r="G88" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H88" s="12"/>
       <c r="I88" s="12"/>
@@ -18579,7 +18617,7 @@
         <v>1</v>
       </c>
       <c r="G89" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H89" s="12"/>
       <c r="I89" s="12"/>
@@ -18609,7 +18647,7 @@
         <v>1</v>
       </c>
       <c r="G90" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="12"/>
@@ -18639,7 +18677,7 @@
         <v>1</v>
       </c>
       <c r="G91" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="12"/>
@@ -18669,7 +18707,7 @@
         <v>1</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H92" s="12"/>
       <c r="I92" s="12"/>
@@ -18699,7 +18737,7 @@
         <v>1</v>
       </c>
       <c r="G93" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H93" s="12"/>
       <c r="I93" s="12"/>
@@ -18729,7 +18767,7 @@
         <v>1</v>
       </c>
       <c r="G94" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H94" s="12"/>
       <c r="I94" s="12"/>
@@ -18759,7 +18797,7 @@
         <v>1</v>
       </c>
       <c r="G95" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="12"/>
@@ -18789,7 +18827,7 @@
         <v>1</v>
       </c>
       <c r="G96" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H96" s="12"/>
       <c r="I96" s="12"/>
@@ -18819,7 +18857,7 @@
         <v>1</v>
       </c>
       <c r="G97" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H97" s="12"/>
       <c r="I97" s="12"/>
@@ -18849,7 +18887,7 @@
         <v>1</v>
       </c>
       <c r="G98" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H98" s="12"/>
       <c r="I98" s="12"/>
@@ -18879,7 +18917,7 @@
         <v>1</v>
       </c>
       <c r="G99" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H99" s="12"/>
       <c r="I99" s="12"/>
@@ -18909,7 +18947,7 @@
         <v>1</v>
       </c>
       <c r="G100" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H100" s="12"/>
       <c r="I100" s="12"/>
@@ -18939,7 +18977,7 @@
         <v>1</v>
       </c>
       <c r="G101" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H101" s="12"/>
       <c r="I101" s="12"/>
@@ -18969,7 +19007,7 @@
         <v>1</v>
       </c>
       <c r="G102" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H102" s="12"/>
       <c r="I102" s="12"/>
@@ -18999,7 +19037,7 @@
         <v>1</v>
       </c>
       <c r="G103" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H103" s="12"/>
       <c r="I103" s="12"/>
@@ -19029,7 +19067,7 @@
         <v>1</v>
       </c>
       <c r="G104" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
@@ -19059,7 +19097,7 @@
         <v>1</v>
       </c>
       <c r="G105" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H105" s="12"/>
       <c r="I105" s="12"/>
@@ -19089,7 +19127,7 @@
         <v>1</v>
       </c>
       <c r="G106" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
@@ -19119,7 +19157,7 @@
         <v>1</v>
       </c>
       <c r="G107" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
@@ -19149,7 +19187,7 @@
         <v>1</v>
       </c>
       <c r="G108" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
@@ -19179,7 +19217,7 @@
         <v>1</v>
       </c>
       <c r="G109" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
@@ -19209,7 +19247,7 @@
         <v>1</v>
       </c>
       <c r="G110" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
@@ -19239,7 +19277,7 @@
         <v>1</v>
       </c>
       <c r="G111" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
@@ -19269,7 +19307,7 @@
         <v>1</v>
       </c>
       <c r="G112" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
@@ -19299,7 +19337,7 @@
         <v>1</v>
       </c>
       <c r="G113" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
@@ -19329,7 +19367,7 @@
         <v>1</v>
       </c>
       <c r="G114" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
@@ -19359,7 +19397,7 @@
         <v>1</v>
       </c>
       <c r="G115" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H115" s="12"/>
       <c r="I115" s="12"/>
@@ -19389,7 +19427,7 @@
         <v>1</v>
       </c>
       <c r="G116" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H116" s="12"/>
       <c r="I116" s="12"/>
@@ -19419,7 +19457,7 @@
         <v>1</v>
       </c>
       <c r="G117" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
@@ -19449,7 +19487,7 @@
         <v>1</v>
       </c>
       <c r="G118" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H118" s="12"/>
       <c r="I118" s="12"/>
@@ -19479,7 +19517,7 @@
         <v>1</v>
       </c>
       <c r="G119" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H119" s="12"/>
       <c r="I119" s="12"/>
@@ -19509,7 +19547,7 @@
         <v>1</v>
       </c>
       <c r="G120" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H120" s="12"/>
       <c r="I120" s="12"/>
@@ -19539,7 +19577,7 @@
         <v>1</v>
       </c>
       <c r="G121" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H121" s="12"/>
       <c r="I121" s="12"/>
@@ -19569,7 +19607,7 @@
         <v>1</v>
       </c>
       <c r="G122" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H122" s="12"/>
       <c r="I122" s="12"/>
@@ -19599,7 +19637,7 @@
         <v>1</v>
       </c>
       <c r="G123" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H123" s="12"/>
       <c r="I123" s="12"/>
@@ -19629,7 +19667,7 @@
         <v>1</v>
       </c>
       <c r="G124" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H124" s="12"/>
       <c r="I124" s="12"/>
@@ -19659,7 +19697,7 @@
         <v>1</v>
       </c>
       <c r="G125" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H125" s="12"/>
       <c r="I125" s="12"/>
@@ -19689,7 +19727,7 @@
         <v>1</v>
       </c>
       <c r="G126" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H126" s="12"/>
       <c r="I126" s="12"/>
@@ -19719,7 +19757,7 @@
         <v>1</v>
       </c>
       <c r="G127" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H127" s="12"/>
       <c r="I127" s="12"/>
@@ -19749,7 +19787,7 @@
         <v>1</v>
       </c>
       <c r="G128" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H128" s="12"/>
       <c r="I128" s="12"/>
@@ -19779,7 +19817,7 @@
         <v>1</v>
       </c>
       <c r="G129" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H129" s="12"/>
       <c r="I129" s="12"/>
@@ -19809,7 +19847,7 @@
         <v>1</v>
       </c>
       <c r="G130" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H130" s="12"/>
       <c r="I130" s="12"/>
@@ -19839,7 +19877,7 @@
         <v>1</v>
       </c>
       <c r="G131" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H131" s="12"/>
       <c r="I131" s="12"/>
@@ -19869,7 +19907,7 @@
         <v>1</v>
       </c>
       <c r="G132" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H132" s="12"/>
       <c r="I132" s="12"/>
@@ -19899,7 +19937,7 @@
         <v>1</v>
       </c>
       <c r="G133" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H133" s="12"/>
       <c r="I133" s="12"/>
@@ -19929,7 +19967,7 @@
         <v>1</v>
       </c>
       <c r="G134" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H134" s="12"/>
       <c r="I134" s="12"/>
@@ -19959,7 +19997,7 @@
         <v>1</v>
       </c>
       <c r="G135" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H135" s="12"/>
       <c r="I135" s="12"/>
@@ -19989,7 +20027,7 @@
         <v>1</v>
       </c>
       <c r="G136" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H136" s="12"/>
       <c r="I136" s="12"/>
@@ -20019,7 +20057,7 @@
         <v>1</v>
       </c>
       <c r="G137" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H137" s="12"/>
       <c r="I137" s="12"/>
@@ -20047,7 +20085,7 @@
     </row>
     <row r="139">
       <c r="A139" s="16" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B139" s="16"/>
       <c r="C139" s="16"/>
@@ -20073,17 +20111,17 @@
       <c r="C140" s="12">
         <v>10000000</v>
       </c>
-      <c r="D140" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E140" s="26" t="s">
-        <v>144</v>
+      <c r="D140" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E140" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="F140" s="20">
         <v>1</v>
       </c>
       <c r="G140" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H140" s="12"/>
       <c r="I140" s="12"/>
@@ -20095,7 +20133,7 @@
     </row>
     <row r="141">
       <c r="A141" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
@@ -20116,7 +20154,7 @@
         <v>255</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C142" s="12">
         <v>11111111</v>

</xml_diff>

<commit_message>
sw - water level rozpracovano
</commit_message>
<xml_diff>
--- a/sw/CAN_Adresses.xlsx
+++ b/sw/CAN_Adresses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t xml:space="preserve">SID bits</t>
   </si>
@@ -291,13 +291,25 @@
     <t xml:space="preserve">"To master" general commands definition</t>
   </si>
   <si>
+    <t>Payload[1]</t>
+  </si>
+  <si>
+    <t>Payload[2+]</t>
+  </si>
+  <si>
     <t>0b010xxxxxxxx</t>
   </si>
   <si>
     <t xml:space="preserve">TM CMD number</t>
   </si>
   <si>
+    <t xml:space="preserve">Operation status</t>
+  </si>
+  <si>
     <t xml:space="preserve">where xx... is slave address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the case of the  error these bytes cound not be send</t>
   </si>
   <si>
     <t>CAN_TM_RST_RES</t>
@@ -307,6 +319,9 @@
   </si>
   <si>
     <t xml:space="preserve">fixed, CMD num.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed, status</t>
   </si>
   <si>
     <t>CAN_TM_RES_DEF_RES</t>
@@ -369,7 +384,7 @@
     <t xml:space="preserve">Get node uptime response</t>
   </si>
   <si>
-    <t xml:space="preserve">Uptime in ms - 7 bytes</t>
+    <t xml:space="preserve">Uptime in ms - 6 bytes</t>
   </si>
   <si>
     <t>CAN_TM_GET_FW_VER_RES</t>
@@ -647,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -679,8 +694,17 @@
     <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="3" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
@@ -692,8 +716,7 @@
     <xf fontId="0" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf fontId="0" fillId="3" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="3" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -708,8 +731,15 @@
       <alignment horizontal="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8941,7 +8971,7 @@
     <col customWidth="1" min="5" max="5" width="39.140625"/>
     <col customWidth="1" min="7" max="7" width="18.57421875"/>
     <col customWidth="1" min="8" max="8" width="13.140625"/>
-    <col customWidth="1" min="9" max="9" width="10.421875"/>
+    <col customWidth="1" min="9" max="9" width="12.140625"/>
     <col customWidth="1" min="10" max="11" width="11.140625"/>
   </cols>
   <sheetData>
@@ -8967,26 +8997,32 @@
         <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>91</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5"/>
@@ -8995,10 +9031,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7"/>
+    <row r="7">
+      <c r="I7" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="8" s="2" customFormat="1">
       <c r="A8" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>60</v>
@@ -9057,7 +9097,7 @@
       <c r="N9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="17"/>
+      <c r="O9" s="19"/>
     </row>
     <row r="10">
       <c r="A10" s="10">
@@ -9071,19 +9111,21 @@
         <f t="shared" ref="C10:C73" si="7">DEC2BIN(A10,8)</f>
         <v>00000000</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>94</v>
+      <c r="D10" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="18">
-        <v>1</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" s="18"/>
+        <v>99</v>
+      </c>
+      <c r="F10" s="20">
+        <v>2</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>101</v>
+      </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -9103,19 +9145,21 @@
         <f t="shared" si="7"/>
         <v>00000001</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>97</v>
+      <c r="D11" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" s="20">
-        <v>1</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="20"/>
+        <v>103</v>
+      </c>
+      <c r="F11" s="23">
+        <v>2</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -9135,19 +9179,21 @@
         <f t="shared" si="7"/>
         <v>00000010</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>99</v>
+      <c r="D12" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="E12" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="23">
+        <v>2</v>
+      </c>
+      <c r="G12" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="20">
-        <v>1</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H12" s="20"/>
+      <c r="H12" s="25" t="s">
+        <v>101</v>
+      </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
@@ -9167,19 +9213,21 @@
         <f t="shared" si="7"/>
         <v>00000011</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="23">
+        <v>2</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="20">
-        <v>1</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H13" s="20"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -9199,27 +9247,29 @@
         <f t="shared" si="7"/>
         <v>00000100</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>103</v>
+      <c r="D14" s="23" t="s">
+        <v>108</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="20">
-        <v>5</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+        <v>109</v>
+      </c>
+      <c r="F14" s="23">
+        <v>6</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15">
       <c r="A15" s="12">
@@ -9234,21 +9284,23 @@
         <v>00000101</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="20">
-        <v>2</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="12"/>
+        <v>112</v>
+      </c>
+      <c r="F15" s="23">
+        <v>3</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>113</v>
+      </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
@@ -9268,21 +9320,23 @@
         <v>00000110</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="20">
-        <v>2</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" s="12"/>
+        <v>115</v>
+      </c>
+      <c r="F16" s="23">
+        <v>3</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>116</v>
+      </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
@@ -9302,21 +9356,23 @@
         <v>00000111</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="F17" s="20">
-        <v>2</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="I17" s="12"/>
+        <v>118</v>
+      </c>
+      <c r="F17" s="23">
+        <v>3</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -9336,26 +9392,28 @@
         <v>00001000</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="20">
+        <v>121</v>
+      </c>
+      <c r="F18" s="23">
         <v>8</v>
       </c>
-      <c r="G18" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
+      <c r="G18" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="31"/>
     </row>
     <row r="19">
       <c r="A19" s="12">
@@ -9369,28 +9427,30 @@
         <f t="shared" si="7"/>
         <v>00001001</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>119</v>
+      <c r="D19" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="F19" s="12">
-        <v>4</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="I19" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="J19" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="K19" s="12"/>
+        <v>5</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>127</v>
+      </c>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
@@ -12481,7 +12541,7 @@
     </row>
     <row r="139">
       <c r="A139" s="16" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B139" s="16"/>
       <c r="C139" s="16"/>
@@ -12508,16 +12568,16 @@
         <v>10000000</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E140" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F140" s="20">
+        <v>130</v>
+      </c>
+      <c r="F140" s="23">
         <v>1</v>
       </c>
-      <c r="G140" s="20" t="s">
-        <v>96</v>
+      <c r="G140" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H140" s="12"/>
       <c r="I140" s="12"/>
@@ -16056,7 +16116,7 @@
       <c r="N360" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
@@ -16064,8 +16124,7 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H18:N18"/>
+    <mergeCell ref="I14:L14"/>
     <mergeCell ref="A139:G139"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
@@ -16094,7 +16153,7 @@
   <sheetData>
     <row r="1" ht="21">
       <c r="A1" s="4" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -16119,7 +16178,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -16133,7 +16192,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5"/>
@@ -16218,16 +16277,16 @@
         <v>00000000</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -16250,16 +16309,16 @@
         <v>00000001</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F11" s="12">
         <v>1</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -16282,19 +16341,19 @@
         <v>00000010</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F12" s="12">
         <v>2</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -16316,16 +16375,16 @@
         <v>00000011</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F13" s="12">
         <v>1</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -16348,16 +16407,16 @@
         <v>00000100</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F14" s="20">
+        <v>143</v>
+      </c>
+      <c r="F14" s="23">
         <v>1</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>96</v>
+      <c r="G14" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -16380,16 +16439,16 @@
         <v>00000101</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="F15" s="20">
+        <v>145</v>
+      </c>
+      <c r="F15" s="23">
         <v>1</v>
       </c>
-      <c r="G15" s="20" t="s">
-        <v>96</v>
+      <c r="G15" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -16412,16 +16471,16 @@
         <v>00000110</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="20">
+        <v>147</v>
+      </c>
+      <c r="F16" s="23">
         <v>1</v>
       </c>
-      <c r="G16" s="20" t="s">
-        <v>96</v>
+      <c r="G16" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -16444,16 +16503,16 @@
         <v>00000111</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="F17" s="20">
+        <v>149</v>
+      </c>
+      <c r="F17" s="23">
         <v>1</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>96</v>
+      <c r="G17" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -16476,16 +16535,16 @@
         <v>00001000</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="20">
+        <v>151</v>
+      </c>
+      <c r="F18" s="23">
         <v>1</v>
       </c>
-      <c r="G18" s="20" t="s">
-        <v>96</v>
+      <c r="G18" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -16507,17 +16566,17 @@
         <f t="shared" si="13"/>
         <v>00001001</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="F19" s="20">
+      <c r="D19" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="23">
         <v>1</v>
       </c>
-      <c r="G19" s="20" t="s">
-        <v>96</v>
+      <c r="G19" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -16543,11 +16602,11 @@
       <c r="E20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="23">
         <v>1</v>
       </c>
-      <c r="G20" s="20" t="s">
-        <v>96</v>
+      <c r="G20" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -16573,11 +16632,11 @@
       <c r="E21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="23">
         <v>1</v>
       </c>
-      <c r="G21" s="20" t="s">
-        <v>96</v>
+      <c r="G21" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -16603,11 +16662,11 @@
       <c r="E22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="23">
         <v>1</v>
       </c>
-      <c r="G22" s="20" t="s">
-        <v>96</v>
+      <c r="G22" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -16633,11 +16692,11 @@
       <c r="E23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="23">
         <v>1</v>
       </c>
-      <c r="G23" s="20" t="s">
-        <v>96</v>
+      <c r="G23" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -16663,11 +16722,11 @@
       <c r="E24" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="23">
         <v>1</v>
       </c>
-      <c r="G24" s="20" t="s">
-        <v>96</v>
+      <c r="G24" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -16693,11 +16752,11 @@
       <c r="E25" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="23">
         <v>1</v>
       </c>
-      <c r="G25" s="20" t="s">
-        <v>96</v>
+      <c r="G25" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -16723,11 +16782,11 @@
       <c r="E26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="23">
         <v>1</v>
       </c>
-      <c r="G26" s="20" t="s">
-        <v>96</v>
+      <c r="G26" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -16753,11 +16812,11 @@
       <c r="E27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="23">
         <v>1</v>
       </c>
-      <c r="G27" s="20" t="s">
-        <v>96</v>
+      <c r="G27" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -16783,11 +16842,11 @@
       <c r="E28" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="23">
         <v>1</v>
       </c>
-      <c r="G28" s="20" t="s">
-        <v>96</v>
+      <c r="G28" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -16813,11 +16872,11 @@
       <c r="E29" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="23">
         <v>1</v>
       </c>
-      <c r="G29" s="20" t="s">
-        <v>96</v>
+      <c r="G29" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -16843,11 +16902,11 @@
       <c r="E30" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="23">
         <v>1</v>
       </c>
-      <c r="G30" s="20" t="s">
-        <v>96</v>
+      <c r="G30" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -16873,11 +16932,11 @@
       <c r="E31" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="23">
         <v>1</v>
       </c>
-      <c r="G31" s="20" t="s">
-        <v>96</v>
+      <c r="G31" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -16903,11 +16962,11 @@
       <c r="E32" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="20">
+      <c r="F32" s="23">
         <v>1</v>
       </c>
-      <c r="G32" s="20" t="s">
-        <v>96</v>
+      <c r="G32" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -16933,11 +16992,11 @@
       <c r="E33" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="20">
+      <c r="F33" s="23">
         <v>1</v>
       </c>
-      <c r="G33" s="20" t="s">
-        <v>96</v>
+      <c r="G33" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
@@ -16963,11 +17022,11 @@
       <c r="E34" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="20">
+      <c r="F34" s="23">
         <v>1</v>
       </c>
-      <c r="G34" s="20" t="s">
-        <v>96</v>
+      <c r="G34" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
@@ -16993,11 +17052,11 @@
       <c r="E35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="23">
         <v>1</v>
       </c>
-      <c r="G35" s="20" t="s">
-        <v>96</v>
+      <c r="G35" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
@@ -17023,11 +17082,11 @@
       <c r="E36" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="20">
+      <c r="F36" s="23">
         <v>1</v>
       </c>
-      <c r="G36" s="20" t="s">
-        <v>96</v>
+      <c r="G36" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
@@ -17053,11 +17112,11 @@
       <c r="E37" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="20">
+      <c r="F37" s="23">
         <v>1</v>
       </c>
-      <c r="G37" s="20" t="s">
-        <v>96</v>
+      <c r="G37" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
@@ -17083,11 +17142,11 @@
       <c r="E38" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="20">
+      <c r="F38" s="23">
         <v>1</v>
       </c>
-      <c r="G38" s="20" t="s">
-        <v>96</v>
+      <c r="G38" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
@@ -17113,11 +17172,11 @@
       <c r="E39" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="20">
+      <c r="F39" s="23">
         <v>1</v>
       </c>
-      <c r="G39" s="20" t="s">
-        <v>96</v>
+      <c r="G39" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
@@ -17143,11 +17202,11 @@
       <c r="E40" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="20">
+      <c r="F40" s="23">
         <v>1</v>
       </c>
-      <c r="G40" s="20" t="s">
-        <v>96</v>
+      <c r="G40" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
@@ -17173,11 +17232,11 @@
       <c r="E41" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F41" s="20">
+      <c r="F41" s="23">
         <v>1</v>
       </c>
-      <c r="G41" s="20" t="s">
-        <v>96</v>
+      <c r="G41" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
@@ -17203,11 +17262,11 @@
       <c r="E42" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="20">
+      <c r="F42" s="23">
         <v>1</v>
       </c>
-      <c r="G42" s="20" t="s">
-        <v>96</v>
+      <c r="G42" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
@@ -17233,11 +17292,11 @@
       <c r="E43" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F43" s="20">
+      <c r="F43" s="23">
         <v>1</v>
       </c>
-      <c r="G43" s="20" t="s">
-        <v>96</v>
+      <c r="G43" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
@@ -17263,11 +17322,11 @@
       <c r="E44" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="20">
+      <c r="F44" s="23">
         <v>1</v>
       </c>
-      <c r="G44" s="20" t="s">
-        <v>96</v>
+      <c r="G44" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
@@ -17293,11 +17352,11 @@
       <c r="E45" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F45" s="23">
         <v>1</v>
       </c>
-      <c r="G45" s="20" t="s">
-        <v>96</v>
+      <c r="G45" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
@@ -17323,11 +17382,11 @@
       <c r="E46" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="20">
+      <c r="F46" s="23">
         <v>1</v>
       </c>
-      <c r="G46" s="20" t="s">
-        <v>96</v>
+      <c r="G46" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
@@ -17353,11 +17412,11 @@
       <c r="E47" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F47" s="20">
+      <c r="F47" s="23">
         <v>1</v>
       </c>
-      <c r="G47" s="20" t="s">
-        <v>96</v>
+      <c r="G47" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
@@ -17383,11 +17442,11 @@
       <c r="E48" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="20">
+      <c r="F48" s="23">
         <v>1</v>
       </c>
-      <c r="G48" s="20" t="s">
-        <v>96</v>
+      <c r="G48" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
@@ -17413,11 +17472,11 @@
       <c r="E49" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F49" s="20">
+      <c r="F49" s="23">
         <v>1</v>
       </c>
-      <c r="G49" s="20" t="s">
-        <v>96</v>
+      <c r="G49" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
@@ -17443,11 +17502,11 @@
       <c r="E50" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F50" s="20">
+      <c r="F50" s="23">
         <v>1</v>
       </c>
-      <c r="G50" s="20" t="s">
-        <v>96</v>
+      <c r="G50" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
@@ -17473,11 +17532,11 @@
       <c r="E51" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F51" s="20">
+      <c r="F51" s="23">
         <v>1</v>
       </c>
-      <c r="G51" s="20" t="s">
-        <v>96</v>
+      <c r="G51" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
@@ -17503,11 +17562,11 @@
       <c r="E52" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="23">
         <v>1</v>
       </c>
-      <c r="G52" s="20" t="s">
-        <v>96</v>
+      <c r="G52" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
@@ -17533,11 +17592,11 @@
       <c r="E53" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="20">
+      <c r="F53" s="23">
         <v>1</v>
       </c>
-      <c r="G53" s="20" t="s">
-        <v>96</v>
+      <c r="G53" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
@@ -17563,11 +17622,11 @@
       <c r="E54" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F54" s="20">
+      <c r="F54" s="23">
         <v>1</v>
       </c>
-      <c r="G54" s="20" t="s">
-        <v>96</v>
+      <c r="G54" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
@@ -17593,11 +17652,11 @@
       <c r="E55" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="23">
         <v>1</v>
       </c>
-      <c r="G55" s="20" t="s">
-        <v>96</v>
+      <c r="G55" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
@@ -17623,11 +17682,11 @@
       <c r="E56" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="23">
         <v>1</v>
       </c>
-      <c r="G56" s="20" t="s">
-        <v>96</v>
+      <c r="G56" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
@@ -17653,11 +17712,11 @@
       <c r="E57" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F57" s="23">
         <v>1</v>
       </c>
-      <c r="G57" s="20" t="s">
-        <v>96</v>
+      <c r="G57" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
@@ -17683,11 +17742,11 @@
       <c r="E58" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F58" s="20">
+      <c r="F58" s="23">
         <v>1</v>
       </c>
-      <c r="G58" s="20" t="s">
-        <v>96</v>
+      <c r="G58" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
@@ -17713,11 +17772,11 @@
       <c r="E59" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F59" s="20">
+      <c r="F59" s="23">
         <v>1</v>
       </c>
-      <c r="G59" s="20" t="s">
-        <v>96</v>
+      <c r="G59" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
@@ -17743,11 +17802,11 @@
       <c r="E60" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F60" s="20">
+      <c r="F60" s="23">
         <v>1</v>
       </c>
-      <c r="G60" s="20" t="s">
-        <v>96</v>
+      <c r="G60" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
@@ -17773,11 +17832,11 @@
       <c r="E61" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F61" s="20">
+      <c r="F61" s="23">
         <v>1</v>
       </c>
-      <c r="G61" s="20" t="s">
-        <v>96</v>
+      <c r="G61" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
@@ -17803,11 +17862,11 @@
       <c r="E62" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F62" s="20">
+      <c r="F62" s="23">
         <v>1</v>
       </c>
-      <c r="G62" s="20" t="s">
-        <v>96</v>
+      <c r="G62" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
@@ -17833,11 +17892,11 @@
       <c r="E63" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F63" s="20">
+      <c r="F63" s="23">
         <v>1</v>
       </c>
-      <c r="G63" s="20" t="s">
-        <v>96</v>
+      <c r="G63" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H63" s="12"/>
       <c r="I63" s="12"/>
@@ -17863,11 +17922,11 @@
       <c r="E64" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F64" s="20">
+      <c r="F64" s="23">
         <v>1</v>
       </c>
-      <c r="G64" s="20" t="s">
-        <v>96</v>
+      <c r="G64" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H64" s="12"/>
       <c r="I64" s="12"/>
@@ -17893,11 +17952,11 @@
       <c r="E65" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F65" s="20">
+      <c r="F65" s="23">
         <v>1</v>
       </c>
-      <c r="G65" s="20" t="s">
-        <v>96</v>
+      <c r="G65" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
@@ -17923,11 +17982,11 @@
       <c r="E66" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="20">
+      <c r="F66" s="23">
         <v>1</v>
       </c>
-      <c r="G66" s="20" t="s">
-        <v>96</v>
+      <c r="G66" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
@@ -17953,11 +18012,11 @@
       <c r="E67" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F67" s="20">
+      <c r="F67" s="23">
         <v>1</v>
       </c>
-      <c r="G67" s="20" t="s">
-        <v>96</v>
+      <c r="G67" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
@@ -17983,11 +18042,11 @@
       <c r="E68" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F68" s="20">
+      <c r="F68" s="23">
         <v>1</v>
       </c>
-      <c r="G68" s="20" t="s">
-        <v>96</v>
+      <c r="G68" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H68" s="12"/>
       <c r="I68" s="12"/>
@@ -18013,11 +18072,11 @@
       <c r="E69" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F69" s="20">
+      <c r="F69" s="23">
         <v>1</v>
       </c>
-      <c r="G69" s="20" t="s">
-        <v>96</v>
+      <c r="G69" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
@@ -18043,11 +18102,11 @@
       <c r="E70" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F70" s="20">
+      <c r="F70" s="23">
         <v>1</v>
       </c>
-      <c r="G70" s="20" t="s">
-        <v>96</v>
+      <c r="G70" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H70" s="12"/>
       <c r="I70" s="12"/>
@@ -18073,11 +18132,11 @@
       <c r="E71" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F71" s="20">
+      <c r="F71" s="23">
         <v>1</v>
       </c>
-      <c r="G71" s="20" t="s">
-        <v>96</v>
+      <c r="G71" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="12"/>
@@ -18103,11 +18162,11 @@
       <c r="E72" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F72" s="20">
+      <c r="F72" s="23">
         <v>1</v>
       </c>
-      <c r="G72" s="20" t="s">
-        <v>96</v>
+      <c r="G72" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H72" s="12"/>
       <c r="I72" s="12"/>
@@ -18133,11 +18192,11 @@
       <c r="E73" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F73" s="20">
+      <c r="F73" s="23">
         <v>1</v>
       </c>
-      <c r="G73" s="20" t="s">
-        <v>96</v>
+      <c r="G73" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H73" s="12"/>
       <c r="I73" s="12"/>
@@ -18163,11 +18222,11 @@
       <c r="E74" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F74" s="20">
+      <c r="F74" s="23">
         <v>1</v>
       </c>
-      <c r="G74" s="20" t="s">
-        <v>96</v>
+      <c r="G74" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H74" s="12"/>
       <c r="I74" s="12"/>
@@ -18193,11 +18252,11 @@
       <c r="E75" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F75" s="20">
+      <c r="F75" s="23">
         <v>1</v>
       </c>
-      <c r="G75" s="20" t="s">
-        <v>96</v>
+      <c r="G75" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H75" s="12"/>
       <c r="I75" s="12"/>
@@ -18223,11 +18282,11 @@
       <c r="E76" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F76" s="20">
+      <c r="F76" s="23">
         <v>1</v>
       </c>
-      <c r="G76" s="20" t="s">
-        <v>96</v>
+      <c r="G76" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H76" s="12"/>
       <c r="I76" s="12"/>
@@ -18253,11 +18312,11 @@
       <c r="E77" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F77" s="20">
+      <c r="F77" s="23">
         <v>1</v>
       </c>
-      <c r="G77" s="20" t="s">
-        <v>96</v>
+      <c r="G77" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H77" s="12"/>
       <c r="I77" s="12"/>
@@ -18283,11 +18342,11 @@
       <c r="E78" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F78" s="20">
+      <c r="F78" s="23">
         <v>1</v>
       </c>
-      <c r="G78" s="20" t="s">
-        <v>96</v>
+      <c r="G78" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H78" s="12"/>
       <c r="I78" s="12"/>
@@ -18313,11 +18372,11 @@
       <c r="E79" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F79" s="20">
+      <c r="F79" s="23">
         <v>1</v>
       </c>
-      <c r="G79" s="20" t="s">
-        <v>96</v>
+      <c r="G79" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
@@ -18343,11 +18402,11 @@
       <c r="E80" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F80" s="20">
+      <c r="F80" s="23">
         <v>1</v>
       </c>
-      <c r="G80" s="20" t="s">
-        <v>96</v>
+      <c r="G80" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H80" s="12"/>
       <c r="I80" s="12"/>
@@ -18373,11 +18432,11 @@
       <c r="E81" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F81" s="20">
+      <c r="F81" s="23">
         <v>1</v>
       </c>
-      <c r="G81" s="20" t="s">
-        <v>96</v>
+      <c r="G81" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H81" s="12"/>
       <c r="I81" s="12"/>
@@ -18403,11 +18462,11 @@
       <c r="E82" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F82" s="20">
+      <c r="F82" s="23">
         <v>1</v>
       </c>
-      <c r="G82" s="20" t="s">
-        <v>96</v>
+      <c r="G82" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H82" s="12"/>
       <c r="I82" s="12"/>
@@ -18433,11 +18492,11 @@
       <c r="E83" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F83" s="20">
+      <c r="F83" s="23">
         <v>1</v>
       </c>
-      <c r="G83" s="20" t="s">
-        <v>96</v>
+      <c r="G83" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="12"/>
@@ -18463,11 +18522,11 @@
       <c r="E84" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F84" s="20">
+      <c r="F84" s="23">
         <v>1</v>
       </c>
-      <c r="G84" s="20" t="s">
-        <v>96</v>
+      <c r="G84" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="12"/>
@@ -18493,11 +18552,11 @@
       <c r="E85" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F85" s="20">
+      <c r="F85" s="23">
         <v>1</v>
       </c>
-      <c r="G85" s="20" t="s">
-        <v>96</v>
+      <c r="G85" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H85" s="12"/>
       <c r="I85" s="12"/>
@@ -18523,11 +18582,11 @@
       <c r="E86" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F86" s="20">
+      <c r="F86" s="23">
         <v>1</v>
       </c>
-      <c r="G86" s="20" t="s">
-        <v>96</v>
+      <c r="G86" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H86" s="12"/>
       <c r="I86" s="12"/>
@@ -18553,11 +18612,11 @@
       <c r="E87" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F87" s="20">
+      <c r="F87" s="23">
         <v>1</v>
       </c>
-      <c r="G87" s="20" t="s">
-        <v>96</v>
+      <c r="G87" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H87" s="12"/>
       <c r="I87" s="12"/>
@@ -18583,11 +18642,11 @@
       <c r="E88" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F88" s="20">
+      <c r="F88" s="23">
         <v>1</v>
       </c>
-      <c r="G88" s="20" t="s">
-        <v>96</v>
+      <c r="G88" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H88" s="12"/>
       <c r="I88" s="12"/>
@@ -18613,11 +18672,11 @@
       <c r="E89" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F89" s="20">
+      <c r="F89" s="23">
         <v>1</v>
       </c>
-      <c r="G89" s="20" t="s">
-        <v>96</v>
+      <c r="G89" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H89" s="12"/>
       <c r="I89" s="12"/>
@@ -18643,11 +18702,11 @@
       <c r="E90" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F90" s="20">
+      <c r="F90" s="23">
         <v>1</v>
       </c>
-      <c r="G90" s="20" t="s">
-        <v>96</v>
+      <c r="G90" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="12"/>
@@ -18673,11 +18732,11 @@
       <c r="E91" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F91" s="20">
+      <c r="F91" s="23">
         <v>1</v>
       </c>
-      <c r="G91" s="20" t="s">
-        <v>96</v>
+      <c r="G91" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="12"/>
@@ -18703,11 +18762,11 @@
       <c r="E92" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F92" s="20">
+      <c r="F92" s="23">
         <v>1</v>
       </c>
-      <c r="G92" s="20" t="s">
-        <v>96</v>
+      <c r="G92" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H92" s="12"/>
       <c r="I92" s="12"/>
@@ -18733,11 +18792,11 @@
       <c r="E93" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F93" s="20">
+      <c r="F93" s="23">
         <v>1</v>
       </c>
-      <c r="G93" s="20" t="s">
-        <v>96</v>
+      <c r="G93" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H93" s="12"/>
       <c r="I93" s="12"/>
@@ -18763,11 +18822,11 @@
       <c r="E94" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F94" s="20">
+      <c r="F94" s="23">
         <v>1</v>
       </c>
-      <c r="G94" s="20" t="s">
-        <v>96</v>
+      <c r="G94" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H94" s="12"/>
       <c r="I94" s="12"/>
@@ -18793,11 +18852,11 @@
       <c r="E95" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F95" s="20">
+      <c r="F95" s="23">
         <v>1</v>
       </c>
-      <c r="G95" s="20" t="s">
-        <v>96</v>
+      <c r="G95" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="12"/>
@@ -18823,11 +18882,11 @@
       <c r="E96" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F96" s="20">
+      <c r="F96" s="23">
         <v>1</v>
       </c>
-      <c r="G96" s="20" t="s">
-        <v>96</v>
+      <c r="G96" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H96" s="12"/>
       <c r="I96" s="12"/>
@@ -18853,11 +18912,11 @@
       <c r="E97" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F97" s="20">
+      <c r="F97" s="23">
         <v>1</v>
       </c>
-      <c r="G97" s="20" t="s">
-        <v>96</v>
+      <c r="G97" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H97" s="12"/>
       <c r="I97" s="12"/>
@@ -18883,11 +18942,11 @@
       <c r="E98" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F98" s="20">
+      <c r="F98" s="23">
         <v>1</v>
       </c>
-      <c r="G98" s="20" t="s">
-        <v>96</v>
+      <c r="G98" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H98" s="12"/>
       <c r="I98" s="12"/>
@@ -18913,11 +18972,11 @@
       <c r="E99" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F99" s="20">
+      <c r="F99" s="23">
         <v>1</v>
       </c>
-      <c r="G99" s="20" t="s">
-        <v>96</v>
+      <c r="G99" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H99" s="12"/>
       <c r="I99" s="12"/>
@@ -18943,11 +19002,11 @@
       <c r="E100" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F100" s="20">
+      <c r="F100" s="23">
         <v>1</v>
       </c>
-      <c r="G100" s="20" t="s">
-        <v>96</v>
+      <c r="G100" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H100" s="12"/>
       <c r="I100" s="12"/>
@@ -18973,11 +19032,11 @@
       <c r="E101" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F101" s="20">
+      <c r="F101" s="23">
         <v>1</v>
       </c>
-      <c r="G101" s="20" t="s">
-        <v>96</v>
+      <c r="G101" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H101" s="12"/>
       <c r="I101" s="12"/>
@@ -19003,11 +19062,11 @@
       <c r="E102" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F102" s="20">
+      <c r="F102" s="23">
         <v>1</v>
       </c>
-      <c r="G102" s="20" t="s">
-        <v>96</v>
+      <c r="G102" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H102" s="12"/>
       <c r="I102" s="12"/>
@@ -19033,11 +19092,11 @@
       <c r="E103" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F103" s="20">
+      <c r="F103" s="23">
         <v>1</v>
       </c>
-      <c r="G103" s="20" t="s">
-        <v>96</v>
+      <c r="G103" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H103" s="12"/>
       <c r="I103" s="12"/>
@@ -19063,11 +19122,11 @@
       <c r="E104" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F104" s="20">
+      <c r="F104" s="23">
         <v>1</v>
       </c>
-      <c r="G104" s="20" t="s">
-        <v>96</v>
+      <c r="G104" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
@@ -19093,11 +19152,11 @@
       <c r="E105" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F105" s="20">
+      <c r="F105" s="23">
         <v>1</v>
       </c>
-      <c r="G105" s="20" t="s">
-        <v>96</v>
+      <c r="G105" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H105" s="12"/>
       <c r="I105" s="12"/>
@@ -19123,11 +19182,11 @@
       <c r="E106" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F106" s="20">
+      <c r="F106" s="23">
         <v>1</v>
       </c>
-      <c r="G106" s="20" t="s">
-        <v>96</v>
+      <c r="G106" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
@@ -19153,11 +19212,11 @@
       <c r="E107" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F107" s="20">
+      <c r="F107" s="23">
         <v>1</v>
       </c>
-      <c r="G107" s="20" t="s">
-        <v>96</v>
+      <c r="G107" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
@@ -19183,11 +19242,11 @@
       <c r="E108" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F108" s="20">
+      <c r="F108" s="23">
         <v>1</v>
       </c>
-      <c r="G108" s="20" t="s">
-        <v>96</v>
+      <c r="G108" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
@@ -19213,11 +19272,11 @@
       <c r="E109" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F109" s="20">
+      <c r="F109" s="23">
         <v>1</v>
       </c>
-      <c r="G109" s="20" t="s">
-        <v>96</v>
+      <c r="G109" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
@@ -19243,11 +19302,11 @@
       <c r="E110" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F110" s="20">
+      <c r="F110" s="23">
         <v>1</v>
       </c>
-      <c r="G110" s="20" t="s">
-        <v>96</v>
+      <c r="G110" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
@@ -19273,11 +19332,11 @@
       <c r="E111" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F111" s="20">
+      <c r="F111" s="23">
         <v>1</v>
       </c>
-      <c r="G111" s="20" t="s">
-        <v>96</v>
+      <c r="G111" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
@@ -19303,11 +19362,11 @@
       <c r="E112" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F112" s="20">
+      <c r="F112" s="23">
         <v>1</v>
       </c>
-      <c r="G112" s="20" t="s">
-        <v>96</v>
+      <c r="G112" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
@@ -19333,11 +19392,11 @@
       <c r="E113" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F113" s="20">
+      <c r="F113" s="23">
         <v>1</v>
       </c>
-      <c r="G113" s="20" t="s">
-        <v>96</v>
+      <c r="G113" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
@@ -19363,11 +19422,11 @@
       <c r="E114" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F114" s="20">
+      <c r="F114" s="23">
         <v>1</v>
       </c>
-      <c r="G114" s="20" t="s">
-        <v>96</v>
+      <c r="G114" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
@@ -19393,11 +19452,11 @@
       <c r="E115" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F115" s="20">
+      <c r="F115" s="23">
         <v>1</v>
       </c>
-      <c r="G115" s="20" t="s">
-        <v>96</v>
+      <c r="G115" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H115" s="12"/>
       <c r="I115" s="12"/>
@@ -19423,11 +19482,11 @@
       <c r="E116" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F116" s="20">
+      <c r="F116" s="23">
         <v>1</v>
       </c>
-      <c r="G116" s="20" t="s">
-        <v>96</v>
+      <c r="G116" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H116" s="12"/>
       <c r="I116" s="12"/>
@@ -19453,11 +19512,11 @@
       <c r="E117" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F117" s="20">
+      <c r="F117" s="23">
         <v>1</v>
       </c>
-      <c r="G117" s="20" t="s">
-        <v>96</v>
+      <c r="G117" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
@@ -19483,11 +19542,11 @@
       <c r="E118" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F118" s="20">
+      <c r="F118" s="23">
         <v>1</v>
       </c>
-      <c r="G118" s="20" t="s">
-        <v>96</v>
+      <c r="G118" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H118" s="12"/>
       <c r="I118" s="12"/>
@@ -19513,11 +19572,11 @@
       <c r="E119" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F119" s="20">
+      <c r="F119" s="23">
         <v>1</v>
       </c>
-      <c r="G119" s="20" t="s">
-        <v>96</v>
+      <c r="G119" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H119" s="12"/>
       <c r="I119" s="12"/>
@@ -19543,11 +19602,11 @@
       <c r="E120" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F120" s="20">
+      <c r="F120" s="23">
         <v>1</v>
       </c>
-      <c r="G120" s="20" t="s">
-        <v>96</v>
+      <c r="G120" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H120" s="12"/>
       <c r="I120" s="12"/>
@@ -19573,11 +19632,11 @@
       <c r="E121" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F121" s="20">
+      <c r="F121" s="23">
         <v>1</v>
       </c>
-      <c r="G121" s="20" t="s">
-        <v>96</v>
+      <c r="G121" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H121" s="12"/>
       <c r="I121" s="12"/>
@@ -19603,11 +19662,11 @@
       <c r="E122" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F122" s="20">
+      <c r="F122" s="23">
         <v>1</v>
       </c>
-      <c r="G122" s="20" t="s">
-        <v>96</v>
+      <c r="G122" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H122" s="12"/>
       <c r="I122" s="12"/>
@@ -19633,11 +19692,11 @@
       <c r="E123" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F123" s="20">
+      <c r="F123" s="23">
         <v>1</v>
       </c>
-      <c r="G123" s="20" t="s">
-        <v>96</v>
+      <c r="G123" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H123" s="12"/>
       <c r="I123" s="12"/>
@@ -19663,11 +19722,11 @@
       <c r="E124" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F124" s="20">
+      <c r="F124" s="23">
         <v>1</v>
       </c>
-      <c r="G124" s="20" t="s">
-        <v>96</v>
+      <c r="G124" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H124" s="12"/>
       <c r="I124" s="12"/>
@@ -19693,11 +19752,11 @@
       <c r="E125" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F125" s="20">
+      <c r="F125" s="23">
         <v>1</v>
       </c>
-      <c r="G125" s="20" t="s">
-        <v>96</v>
+      <c r="G125" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H125" s="12"/>
       <c r="I125" s="12"/>
@@ -19723,11 +19782,11 @@
       <c r="E126" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F126" s="20">
+      <c r="F126" s="23">
         <v>1</v>
       </c>
-      <c r="G126" s="20" t="s">
-        <v>96</v>
+      <c r="G126" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H126" s="12"/>
       <c r="I126" s="12"/>
@@ -19753,11 +19812,11 @@
       <c r="E127" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F127" s="20">
+      <c r="F127" s="23">
         <v>1</v>
       </c>
-      <c r="G127" s="20" t="s">
-        <v>96</v>
+      <c r="G127" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H127" s="12"/>
       <c r="I127" s="12"/>
@@ -19783,11 +19842,11 @@
       <c r="E128" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F128" s="20">
+      <c r="F128" s="23">
         <v>1</v>
       </c>
-      <c r="G128" s="20" t="s">
-        <v>96</v>
+      <c r="G128" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H128" s="12"/>
       <c r="I128" s="12"/>
@@ -19813,11 +19872,11 @@
       <c r="E129" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F129" s="20">
+      <c r="F129" s="23">
         <v>1</v>
       </c>
-      <c r="G129" s="20" t="s">
-        <v>96</v>
+      <c r="G129" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H129" s="12"/>
       <c r="I129" s="12"/>
@@ -19843,11 +19902,11 @@
       <c r="E130" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F130" s="20">
+      <c r="F130" s="23">
         <v>1</v>
       </c>
-      <c r="G130" s="20" t="s">
-        <v>96</v>
+      <c r="G130" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H130" s="12"/>
       <c r="I130" s="12"/>
@@ -19873,11 +19932,11 @@
       <c r="E131" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F131" s="20">
+      <c r="F131" s="23">
         <v>1</v>
       </c>
-      <c r="G131" s="20" t="s">
-        <v>96</v>
+      <c r="G131" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H131" s="12"/>
       <c r="I131" s="12"/>
@@ -19903,11 +19962,11 @@
       <c r="E132" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F132" s="20">
+      <c r="F132" s="23">
         <v>1</v>
       </c>
-      <c r="G132" s="20" t="s">
-        <v>96</v>
+      <c r="G132" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H132" s="12"/>
       <c r="I132" s="12"/>
@@ -19933,11 +19992,11 @@
       <c r="E133" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F133" s="20">
+      <c r="F133" s="23">
         <v>1</v>
       </c>
-      <c r="G133" s="20" t="s">
-        <v>96</v>
+      <c r="G133" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H133" s="12"/>
       <c r="I133" s="12"/>
@@ -19963,11 +20022,11 @@
       <c r="E134" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F134" s="20">
+      <c r="F134" s="23">
         <v>1</v>
       </c>
-      <c r="G134" s="20" t="s">
-        <v>96</v>
+      <c r="G134" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H134" s="12"/>
       <c r="I134" s="12"/>
@@ -19993,11 +20052,11 @@
       <c r="E135" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F135" s="20">
+      <c r="F135" s="23">
         <v>1</v>
       </c>
-      <c r="G135" s="20" t="s">
-        <v>96</v>
+      <c r="G135" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H135" s="12"/>
       <c r="I135" s="12"/>
@@ -20023,11 +20082,11 @@
       <c r="E136" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F136" s="20">
+      <c r="F136" s="23">
         <v>1</v>
       </c>
-      <c r="G136" s="20" t="s">
-        <v>96</v>
+      <c r="G136" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H136" s="12"/>
       <c r="I136" s="12"/>
@@ -20053,11 +20112,11 @@
       <c r="E137" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F137" s="20">
+      <c r="F137" s="23">
         <v>1</v>
       </c>
-      <c r="G137" s="20" t="s">
-        <v>96</v>
+      <c r="G137" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H137" s="12"/>
       <c r="I137" s="12"/>
@@ -20085,7 +20144,7 @@
     </row>
     <row r="139">
       <c r="A139" s="16" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B139" s="16"/>
       <c r="C139" s="16"/>
@@ -20112,16 +20171,16 @@
         <v>10000000</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E140" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="F140" s="20">
+        <v>156</v>
+      </c>
+      <c r="F140" s="23">
         <v>1</v>
       </c>
-      <c r="G140" s="20" t="s">
-        <v>96</v>
+      <c r="G140" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H140" s="12"/>
       <c r="I140" s="12"/>

</xml_diff>